<commit_message>
Finalizado a leitura do comprovantes de pagamento, alterado as funcao de tratar numeros int e float pra considerar quando o numero já for um int ou float, e melhorado a regra de comparacao no ComparaWithSettings
</commit_message>
<xml_diff>
--- a/backend/accounting_integration/data/configuracoes.xlsx
+++ b/backend/accounting_integration/data/configuracoes.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD19F9F-16E8-45B3-88F8-8ECAB097FB1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FornecedorOuDespesa" sheetId="1" r:id="rId1"/>
     <sheet name="Bancos" sheetId="2" r:id="rId2"/>
     <sheet name="ExtratoBancario" sheetId="4" r:id="rId3"/>
-    <sheet name="DeParaPlanoContas" sheetId="5" r:id="rId4"/>
+    <sheet name="ContasEHistoricoOutros" sheetId="6" r:id="rId4"/>
+    <sheet name="DeParaPlanoContas" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">DeParaPlanoContas!$A$1:$D$3230</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DeParaPlanoContas!$A$1:$D$3230</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Quando no Campo</t>
   </si>
@@ -54,11 +56,35 @@
   <si>
     <t>Nome da Conta Sistema Cliente</t>
   </si>
+  <si>
+    <t>Quando houver</t>
+  </si>
+  <si>
+    <t>na Domínio o código do(a)</t>
+  </si>
+  <si>
+    <t>Será o</t>
+  </si>
+  <si>
+    <t>Juros</t>
+  </si>
+  <si>
+    <t>Histórico</t>
+  </si>
+  <si>
+    <t>Multa</t>
+  </si>
+  <si>
+    <t>Desconto</t>
+  </si>
+  <si>
+    <t>Conta Contábil</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,7 +189,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +227,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -236,6 +262,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -271,9 +314,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,12 +506,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,10 +538,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Conter as palavras,For igual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Fornecedor,Plano de Contas,Categoria,Histórico"</formula1>
     </dataValidation>
   </dataValidations>
@@ -491,7 +551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -519,7 +579,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"DINHEIRO,CEF,BRASIL,ITAU,SICOOB,BRADESCO,SICRED,SANTANDER,SAFRA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -528,12 +588,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,16 +627,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Conter as palavras,For igual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Histórico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Soma,Subtrai,Ambos"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"Soma,Subtrai"</formula1>
     </dataValidation>
   </dataValidations>
@@ -586,7 +646,117 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A97FAF-E9E0-43CA-BDE6-DA88E4E368A3}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8" xr:uid="{69E9F142-A20A-410E-96D5-BAF69D8CE33F}">
+      <formula1>"Juros,Multa,Desconto"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{C913D7FB-8E54-4ABF-9FDA-4CE6FEE0BCBE}">
+      <formula1>"Histórico,Conta Contábil"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10835,7 +11005,7 @@
       <c r="D3230" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D3230"/>
+  <autoFilter ref="A1:D3230" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementado pra ler a estrutura da empresa Center Sol, a lógica é o mesmo da Faaftech, mesmo sistema financeiro.
</commit_message>
<xml_diff>
--- a/backend/accounting_integration/data/configuracoes.xlsx
+++ b/backend/accounting_integration/data/configuracoes.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD19F9F-16E8-45B3-88F8-8ECAB097FB1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FornecedorOuDespesa" sheetId="1" r:id="rId1"/>
@@ -84,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,7 +188,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,7 +226,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -262,23 +261,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -314,26 +296,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -506,7 +471,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -538,10 +503,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000">
       <formula1>"Conter as palavras,For igual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
       <formula1>"Fornecedor,Plano de Contas,Categoria,Histórico"</formula1>
     </dataValidation>
   </dataValidations>
@@ -551,12 +516,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +544,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2:A1001">
       <formula1>"DINHEIRO,CEF,BRASIL,ITAU,SICOOB,BRADESCO,SICRED,SANTANDER,SAFRA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -588,7 +553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -627,16 +592,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000">
       <formula1>"Conter as palavras,For igual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
       <formula1>"Histórico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000">
       <formula1>"Soma,Subtrai,Ambos"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000">
       <formula1>"Soma,Subtrai"</formula1>
     </dataValidation>
   </dataValidations>
@@ -646,10 +611,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A97FAF-E9E0-43CA-BDE6-DA88E4E368A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -744,10 +709,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8" xr:uid="{69E9F142-A20A-410E-96D5-BAF69D8CE33F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8">
       <formula1>"Juros,Multa,Desconto"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{C913D7FB-8E54-4ABF-9FDA-4CE6FEE0BCBE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8">
       <formula1>"Histórico,Conta Contábil"</formula1>
     </dataValidation>
   </dataValidations>
@@ -756,7 +721,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11005,7 +10970,7 @@
       <c r="D3230" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D3230" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:D3230"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Incluindo pro Livro Caixa exportar pra Domínio
</commit_message>
<xml_diff>
--- a/backend/accounting_integration/data/configuracoes.xlsx
+++ b/backend/accounting_integration/data/configuracoes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Quando no Campo</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Conta Contábil</t>
+  </si>
+  <si>
+    <t>Comparar Com</t>
   </si>
 </sst>
 </file>
@@ -517,35 +520,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="A2:A1001">
+  <dataConsolidate/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B2:B1001">
       <formula1>"DINHEIRO,CEF,BRASIL,ITAU,SICOOB,BRADESCO,SICRED,SANTANDER,SAFRA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
+      <formula1>"Extrato Bancário,Financeiro do Cliente"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Adicionado a opção de configurar o de-para do banco e financeiro de uma vez só
</commit_message>
<xml_diff>
--- a/backend/accounting_integration/data/configuracoes.xlsx
+++ b/backend/accounting_integration/data/configuracoes.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50600EF5-01BA-491A-8DB8-EC4BA2BAA181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-20610" yWindow="-945" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FornecedorOuDespesa" sheetId="1" r:id="rId1"/>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,7 +192,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -229,7 +230,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -264,6 +265,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -299,9 +317,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -474,7 +509,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -506,10 +541,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Conter as palavras,For igual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Fornecedor,Plano de Contas,Categoria,Histórico"</formula1>
     </dataValidation>
   </dataValidations>
@@ -519,12 +554,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A998" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1000" sqref="A1000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,11 +587,11 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B2:B1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B2:B1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"DINHEIRO,CEF,BRASIL,ITAU,SICOOB,BRADESCO,SICRED,SANTANDER,SAFRA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
-      <formula1>"Extrato Bancário,Financeiro do Cliente"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{6623F0EB-AD82-4B36-A4CA-ACEF96D8F6FB}">
+      <formula1>"Extrato Bancário,Financeiro do Cliente,Financeiro OU Extrato"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -564,7 +599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -603,16 +638,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Conter as palavras,For igual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Histórico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Soma,Subtrai,Ambos"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"Soma,Subtrai"</formula1>
     </dataValidation>
   </dataValidations>
@@ -622,7 +657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -720,10 +755,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Juros,Multa,Desconto"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Histórico,Conta Contábil"</formula1>
     </dataValidation>
   </dataValidations>
@@ -732,7 +767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D3230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10981,7 +11016,7 @@
       <c r="D3230" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D3230"/>
+  <autoFilter ref="A1:D3230" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementado pra ler o comprovante tipo FGTS-GRRF
</commit_message>
<xml_diff>
--- a/backend/accounting_integration/data/configuracoes.xlsx
+++ b/backend/accounting_integration/data/configuracoes.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50600EF5-01BA-491A-8DB8-EC4BA2BAA181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-945" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-945" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FornecedorOuDespesa" sheetId="1" r:id="rId1"/>
@@ -87,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,7 +191,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -230,7 +229,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -265,23 +264,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -317,26 +299,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -509,7 +474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -541,10 +506,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000">
       <formula1>"Conter as palavras,For igual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
       <formula1>"Fornecedor,Plano de Contas,Categoria,Histórico"</formula1>
     </dataValidation>
   </dataValidations>
@@ -554,12 +519,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A998" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1000" sqref="A1000"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,10 +552,10 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B2:B1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B2:B1001">
       <formula1>"DINHEIRO,CEF,BRASIL,ITAU,SICOOB,BRADESCO,SICRED,SANTANDER,SAFRA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{6623F0EB-AD82-4B36-A4CA-ACEF96D8F6FB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
       <formula1>"Extrato Bancário,Financeiro do Cliente,Financeiro OU Extrato"</formula1>
     </dataValidation>
   </dataValidations>
@@ -599,7 +564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -638,16 +603,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000">
       <formula1>"Conter as palavras,For igual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
       <formula1>"Histórico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1000">
       <formula1>"Soma,Subtrai,Ambos"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000">
       <formula1>"Soma,Subtrai"</formula1>
     </dataValidation>
   </dataValidations>
@@ -657,7 +622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -755,10 +720,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8">
       <formula1>"Juros,Multa,Desconto"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8">
       <formula1>"Histórico,Conta Contábil"</formula1>
     </dataValidation>
   </dataValidations>
@@ -767,7 +732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11016,7 +10981,7 @@
       <c r="D3230" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D3230" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:D3230"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add settings to replace value when field overwriteAccount is Yes. And add | in funcoesUteis
</commit_message>
<xml_diff>
--- a/backend/accounting_integration/data/configuracoes.xlsx
+++ b/backend/accounting_integration/data/configuracoes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Quando no Campo</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Comparar Com</t>
+  </si>
+  <si>
+    <t>Sobrescrever a Conta na Planilha Processada?</t>
   </si>
 </sst>
 </file>
@@ -475,11 +478,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1084"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,9 +491,10 @@
     <col min="2" max="2" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,14 +507,3269 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="2"/>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="2"/>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="2"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="2"/>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E102" s="2"/>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E105" s="2"/>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E106" s="2"/>
+    </row>
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E107" s="2"/>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="2"/>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="2"/>
+    </row>
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E110" s="2"/>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="2"/>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E112" s="2"/>
+    </row>
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E113" s="2"/>
+    </row>
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E114" s="2"/>
+    </row>
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E115" s="2"/>
+    </row>
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E116" s="2"/>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="2"/>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="2"/>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="2"/>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E120" s="2"/>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E121" s="2"/>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="2"/>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="2"/>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="2"/>
+    </row>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E125" s="2"/>
+    </row>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E126" s="2"/>
+    </row>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E127" s="2"/>
+    </row>
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E128" s="2"/>
+    </row>
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E129" s="2"/>
+    </row>
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E130" s="2"/>
+    </row>
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E131" s="2"/>
+    </row>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E132" s="2"/>
+    </row>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E133" s="2"/>
+    </row>
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E134" s="2"/>
+    </row>
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E135" s="2"/>
+    </row>
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E136" s="2"/>
+    </row>
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E137" s="2"/>
+    </row>
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E138" s="2"/>
+    </row>
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E139" s="2"/>
+    </row>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E140" s="2"/>
+    </row>
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E141" s="2"/>
+    </row>
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E142" s="2"/>
+    </row>
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E143" s="2"/>
+    </row>
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E144" s="2"/>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E145" s="2"/>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E146" s="2"/>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E147" s="2"/>
+    </row>
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E148" s="2"/>
+    </row>
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E149" s="2"/>
+    </row>
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E150" s="2"/>
+    </row>
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E151" s="2"/>
+    </row>
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E152" s="2"/>
+    </row>
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E153" s="2"/>
+    </row>
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E154" s="2"/>
+    </row>
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E155" s="2"/>
+    </row>
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E156" s="2"/>
+    </row>
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E157" s="2"/>
+    </row>
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E158" s="2"/>
+    </row>
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E159" s="2"/>
+    </row>
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E160" s="2"/>
+    </row>
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E161" s="2"/>
+    </row>
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E162" s="2"/>
+    </row>
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E163" s="2"/>
+    </row>
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E164" s="2"/>
+    </row>
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E165" s="2"/>
+    </row>
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E166" s="2"/>
+    </row>
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E167" s="2"/>
+    </row>
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E168" s="2"/>
+    </row>
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E169" s="2"/>
+    </row>
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E170" s="2"/>
+    </row>
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E171" s="2"/>
+    </row>
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E172" s="2"/>
+    </row>
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E173" s="2"/>
+    </row>
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E174" s="2"/>
+    </row>
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E175" s="2"/>
+    </row>
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E176" s="2"/>
+    </row>
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E177" s="2"/>
+    </row>
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E178" s="2"/>
+    </row>
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E179" s="2"/>
+    </row>
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E180" s="2"/>
+    </row>
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E181" s="2"/>
+    </row>
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E182" s="2"/>
+    </row>
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E183" s="2"/>
+    </row>
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E184" s="2"/>
+    </row>
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E185" s="2"/>
+    </row>
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E186" s="2"/>
+    </row>
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E187" s="2"/>
+    </row>
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E188" s="2"/>
+    </row>
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E189" s="2"/>
+    </row>
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E190" s="2"/>
+    </row>
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E191" s="2"/>
+    </row>
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E192" s="2"/>
+    </row>
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E193" s="2"/>
+    </row>
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E194" s="2"/>
+    </row>
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E195" s="2"/>
+    </row>
+    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E196" s="2"/>
+    </row>
+    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E197" s="2"/>
+    </row>
+    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E198" s="2"/>
+    </row>
+    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E199" s="2"/>
+    </row>
+    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E200" s="2"/>
+    </row>
+    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E201" s="2"/>
+    </row>
+    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E202" s="2"/>
+    </row>
+    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E203" s="2"/>
+    </row>
+    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E204" s="2"/>
+    </row>
+    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E205" s="2"/>
+    </row>
+    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E206" s="2"/>
+    </row>
+    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E207" s="2"/>
+    </row>
+    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E208" s="2"/>
+    </row>
+    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E209" s="2"/>
+    </row>
+    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E210" s="2"/>
+    </row>
+    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E211" s="2"/>
+    </row>
+    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E212" s="2"/>
+    </row>
+    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E213" s="2"/>
+    </row>
+    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E214" s="2"/>
+    </row>
+    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E215" s="2"/>
+    </row>
+    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E216" s="2"/>
+    </row>
+    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E217" s="2"/>
+    </row>
+    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E218" s="2"/>
+    </row>
+    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E219" s="2"/>
+    </row>
+    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E220" s="2"/>
+    </row>
+    <row r="221" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E221" s="2"/>
+    </row>
+    <row r="222" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E222" s="2"/>
+    </row>
+    <row r="223" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E223" s="2"/>
+    </row>
+    <row r="224" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E224" s="2"/>
+    </row>
+    <row r="225" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E225" s="2"/>
+    </row>
+    <row r="226" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E226" s="2"/>
+    </row>
+    <row r="227" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E227" s="2"/>
+    </row>
+    <row r="228" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E228" s="2"/>
+    </row>
+    <row r="229" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E229" s="2"/>
+    </row>
+    <row r="230" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E230" s="2"/>
+    </row>
+    <row r="231" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E231" s="2"/>
+    </row>
+    <row r="232" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E232" s="2"/>
+    </row>
+    <row r="233" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E233" s="2"/>
+    </row>
+    <row r="234" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E234" s="2"/>
+    </row>
+    <row r="235" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E235" s="2"/>
+    </row>
+    <row r="236" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E236" s="2"/>
+    </row>
+    <row r="237" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E237" s="2"/>
+    </row>
+    <row r="238" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E238" s="2"/>
+    </row>
+    <row r="239" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E239" s="2"/>
+    </row>
+    <row r="240" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E240" s="2"/>
+    </row>
+    <row r="241" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E241" s="2"/>
+    </row>
+    <row r="242" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E242" s="2"/>
+    </row>
+    <row r="243" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E243" s="2"/>
+    </row>
+    <row r="244" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E244" s="2"/>
+    </row>
+    <row r="245" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E245" s="2"/>
+    </row>
+    <row r="246" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E246" s="2"/>
+    </row>
+    <row r="247" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E247" s="2"/>
+    </row>
+    <row r="248" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E248" s="2"/>
+    </row>
+    <row r="249" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E249" s="2"/>
+    </row>
+    <row r="250" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E250" s="2"/>
+    </row>
+    <row r="251" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E251" s="2"/>
+    </row>
+    <row r="252" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E252" s="2"/>
+    </row>
+    <row r="253" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E253" s="2"/>
+    </row>
+    <row r="254" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E254" s="2"/>
+    </row>
+    <row r="255" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E255" s="2"/>
+    </row>
+    <row r="256" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E256" s="2"/>
+    </row>
+    <row r="257" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E257" s="2"/>
+    </row>
+    <row r="258" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E258" s="2"/>
+    </row>
+    <row r="259" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E259" s="2"/>
+    </row>
+    <row r="260" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E260" s="2"/>
+    </row>
+    <row r="261" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E261" s="2"/>
+    </row>
+    <row r="262" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E262" s="2"/>
+    </row>
+    <row r="263" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E263" s="2"/>
+    </row>
+    <row r="264" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E264" s="2"/>
+    </row>
+    <row r="265" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E265" s="2"/>
+    </row>
+    <row r="266" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E266" s="2"/>
+    </row>
+    <row r="267" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E267" s="2"/>
+    </row>
+    <row r="268" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E268" s="2"/>
+    </row>
+    <row r="269" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E269" s="2"/>
+    </row>
+    <row r="270" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E270" s="2"/>
+    </row>
+    <row r="271" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E271" s="2"/>
+    </row>
+    <row r="272" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E272" s="2"/>
+    </row>
+    <row r="273" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E273" s="2"/>
+    </row>
+    <row r="274" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E274" s="2"/>
+    </row>
+    <row r="275" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E275" s="2"/>
+    </row>
+    <row r="276" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E276" s="2"/>
+    </row>
+    <row r="277" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E277" s="2"/>
+    </row>
+    <row r="278" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E278" s="2"/>
+    </row>
+    <row r="279" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E279" s="2"/>
+    </row>
+    <row r="280" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E280" s="2"/>
+    </row>
+    <row r="281" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E281" s="2"/>
+    </row>
+    <row r="282" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E282" s="2"/>
+    </row>
+    <row r="283" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E283" s="2"/>
+    </row>
+    <row r="284" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E284" s="2"/>
+    </row>
+    <row r="285" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E285" s="2"/>
+    </row>
+    <row r="286" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E286" s="2"/>
+    </row>
+    <row r="287" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E287" s="2"/>
+    </row>
+    <row r="288" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E288" s="2"/>
+    </row>
+    <row r="289" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E289" s="2"/>
+    </row>
+    <row r="290" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E290" s="2"/>
+    </row>
+    <row r="291" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E291" s="2"/>
+    </row>
+    <row r="292" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E292" s="2"/>
+    </row>
+    <row r="293" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E293" s="2"/>
+    </row>
+    <row r="294" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E294" s="2"/>
+    </row>
+    <row r="295" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E295" s="2"/>
+    </row>
+    <row r="296" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E296" s="2"/>
+    </row>
+    <row r="297" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E297" s="2"/>
+    </row>
+    <row r="298" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E298" s="2"/>
+    </row>
+    <row r="299" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E299" s="2"/>
+    </row>
+    <row r="300" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E300" s="2"/>
+    </row>
+    <row r="301" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E301" s="2"/>
+    </row>
+    <row r="302" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E302" s="2"/>
+    </row>
+    <row r="303" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E303" s="2"/>
+    </row>
+    <row r="304" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E304" s="2"/>
+    </row>
+    <row r="305" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E305" s="2"/>
+    </row>
+    <row r="306" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E306" s="2"/>
+    </row>
+    <row r="307" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E307" s="2"/>
+    </row>
+    <row r="308" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E308" s="2"/>
+    </row>
+    <row r="309" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E309" s="2"/>
+    </row>
+    <row r="310" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E310" s="2"/>
+    </row>
+    <row r="311" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E311" s="2"/>
+    </row>
+    <row r="312" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E312" s="2"/>
+    </row>
+    <row r="313" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E313" s="2"/>
+    </row>
+    <row r="314" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E314" s="2"/>
+    </row>
+    <row r="315" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E315" s="2"/>
+    </row>
+    <row r="316" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E316" s="2"/>
+    </row>
+    <row r="317" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E317" s="2"/>
+    </row>
+    <row r="318" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E318" s="2"/>
+    </row>
+    <row r="319" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E319" s="2"/>
+    </row>
+    <row r="320" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E320" s="2"/>
+    </row>
+    <row r="321" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E321" s="2"/>
+    </row>
+    <row r="322" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E322" s="2"/>
+    </row>
+    <row r="323" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E323" s="2"/>
+    </row>
+    <row r="324" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E324" s="2"/>
+    </row>
+    <row r="325" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E325" s="2"/>
+    </row>
+    <row r="326" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E326" s="2"/>
+    </row>
+    <row r="327" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E327" s="2"/>
+    </row>
+    <row r="328" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E328" s="2"/>
+    </row>
+    <row r="329" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E329" s="2"/>
+    </row>
+    <row r="330" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E330" s="2"/>
+    </row>
+    <row r="331" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E331" s="2"/>
+    </row>
+    <row r="332" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E332" s="2"/>
+    </row>
+    <row r="333" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E333" s="2"/>
+    </row>
+    <row r="334" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E334" s="2"/>
+    </row>
+    <row r="335" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E335" s="2"/>
+    </row>
+    <row r="336" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E336" s="2"/>
+    </row>
+    <row r="337" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E337" s="2"/>
+    </row>
+    <row r="338" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E338" s="2"/>
+    </row>
+    <row r="339" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E339" s="2"/>
+    </row>
+    <row r="340" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E340" s="2"/>
+    </row>
+    <row r="341" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E341" s="2"/>
+    </row>
+    <row r="342" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E342" s="2"/>
+    </row>
+    <row r="343" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E343" s="2"/>
+    </row>
+    <row r="344" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E344" s="2"/>
+    </row>
+    <row r="345" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E345" s="2"/>
+    </row>
+    <row r="346" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E346" s="2"/>
+    </row>
+    <row r="347" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E347" s="2"/>
+    </row>
+    <row r="348" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E348" s="2"/>
+    </row>
+    <row r="349" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E349" s="2"/>
+    </row>
+    <row r="350" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E350" s="2"/>
+    </row>
+    <row r="351" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E351" s="2"/>
+    </row>
+    <row r="352" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E352" s="2"/>
+    </row>
+    <row r="353" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E353" s="2"/>
+    </row>
+    <row r="354" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E354" s="2"/>
+    </row>
+    <row r="355" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E355" s="2"/>
+    </row>
+    <row r="356" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E356" s="2"/>
+    </row>
+    <row r="357" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E357" s="2"/>
+    </row>
+    <row r="358" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E358" s="2"/>
+    </row>
+    <row r="359" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E359" s="2"/>
+    </row>
+    <row r="360" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E360" s="2"/>
+    </row>
+    <row r="361" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E361" s="2"/>
+    </row>
+    <row r="362" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E362" s="2"/>
+    </row>
+    <row r="363" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E363" s="2"/>
+    </row>
+    <row r="364" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E364" s="2"/>
+    </row>
+    <row r="365" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E365" s="2"/>
+    </row>
+    <row r="366" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E366" s="2"/>
+    </row>
+    <row r="367" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E367" s="2"/>
+    </row>
+    <row r="368" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E368" s="2"/>
+    </row>
+    <row r="369" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E369" s="2"/>
+    </row>
+    <row r="370" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E370" s="2"/>
+    </row>
+    <row r="371" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E371" s="2"/>
+    </row>
+    <row r="372" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E372" s="2"/>
+    </row>
+    <row r="373" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E373" s="2"/>
+    </row>
+    <row r="374" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E374" s="2"/>
+    </row>
+    <row r="375" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E375" s="2"/>
+    </row>
+    <row r="376" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E376" s="2"/>
+    </row>
+    <row r="377" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E377" s="2"/>
+    </row>
+    <row r="378" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E378" s="2"/>
+    </row>
+    <row r="379" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E379" s="2"/>
+    </row>
+    <row r="380" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E380" s="2"/>
+    </row>
+    <row r="381" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E381" s="2"/>
+    </row>
+    <row r="382" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E382" s="2"/>
+    </row>
+    <row r="383" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E383" s="2"/>
+    </row>
+    <row r="384" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E384" s="2"/>
+    </row>
+    <row r="385" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E385" s="2"/>
+    </row>
+    <row r="386" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E386" s="2"/>
+    </row>
+    <row r="387" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E387" s="2"/>
+    </row>
+    <row r="388" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E388" s="2"/>
+    </row>
+    <row r="389" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E389" s="2"/>
+    </row>
+    <row r="390" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E390" s="2"/>
+    </row>
+    <row r="391" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E391" s="2"/>
+    </row>
+    <row r="392" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E392" s="2"/>
+    </row>
+    <row r="393" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E393" s="2"/>
+    </row>
+    <row r="394" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E394" s="2"/>
+    </row>
+    <row r="395" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E395" s="2"/>
+    </row>
+    <row r="396" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E396" s="2"/>
+    </row>
+    <row r="397" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E397" s="2"/>
+    </row>
+    <row r="398" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E398" s="2"/>
+    </row>
+    <row r="399" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E399" s="2"/>
+    </row>
+    <row r="400" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E400" s="2"/>
+    </row>
+    <row r="401" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E401" s="2"/>
+    </row>
+    <row r="402" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E402" s="2"/>
+    </row>
+    <row r="403" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E403" s="2"/>
+    </row>
+    <row r="404" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E404" s="2"/>
+    </row>
+    <row r="405" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E405" s="2"/>
+    </row>
+    <row r="406" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E406" s="2"/>
+    </row>
+    <row r="407" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E407" s="2"/>
+    </row>
+    <row r="408" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E408" s="2"/>
+    </row>
+    <row r="409" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E409" s="2"/>
+    </row>
+    <row r="410" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E410" s="2"/>
+    </row>
+    <row r="411" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E411" s="2"/>
+    </row>
+    <row r="412" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E412" s="2"/>
+    </row>
+    <row r="413" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E413" s="2"/>
+    </row>
+    <row r="414" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E414" s="2"/>
+    </row>
+    <row r="415" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E415" s="2"/>
+    </row>
+    <row r="416" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E416" s="2"/>
+    </row>
+    <row r="417" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E417" s="2"/>
+    </row>
+    <row r="418" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E418" s="2"/>
+    </row>
+    <row r="419" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E419" s="2"/>
+    </row>
+    <row r="420" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E420" s="2"/>
+    </row>
+    <row r="421" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E421" s="2"/>
+    </row>
+    <row r="422" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E422" s="2"/>
+    </row>
+    <row r="423" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E423" s="2"/>
+    </row>
+    <row r="424" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E424" s="2"/>
+    </row>
+    <row r="425" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E425" s="2"/>
+    </row>
+    <row r="426" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E426" s="2"/>
+    </row>
+    <row r="427" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E427" s="2"/>
+    </row>
+    <row r="428" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E428" s="2"/>
+    </row>
+    <row r="429" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E429" s="2"/>
+    </row>
+    <row r="430" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E430" s="2"/>
+    </row>
+    <row r="431" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E431" s="2"/>
+    </row>
+    <row r="432" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E432" s="2"/>
+    </row>
+    <row r="433" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E433" s="2"/>
+    </row>
+    <row r="434" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E434" s="2"/>
+    </row>
+    <row r="435" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E435" s="2"/>
+    </row>
+    <row r="436" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E436" s="2"/>
+    </row>
+    <row r="437" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E437" s="2"/>
+    </row>
+    <row r="438" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E438" s="2"/>
+    </row>
+    <row r="439" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E439" s="2"/>
+    </row>
+    <row r="440" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E440" s="2"/>
+    </row>
+    <row r="441" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E441" s="2"/>
+    </row>
+    <row r="442" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E442" s="2"/>
+    </row>
+    <row r="443" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E443" s="2"/>
+    </row>
+    <row r="444" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E444" s="2"/>
+    </row>
+    <row r="445" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E445" s="2"/>
+    </row>
+    <row r="446" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E446" s="2"/>
+    </row>
+    <row r="447" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E447" s="2"/>
+    </row>
+    <row r="448" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E448" s="2"/>
+    </row>
+    <row r="449" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E449" s="2"/>
+    </row>
+    <row r="450" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E450" s="2"/>
+    </row>
+    <row r="451" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E451" s="2"/>
+    </row>
+    <row r="452" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E452" s="2"/>
+    </row>
+    <row r="453" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E453" s="2"/>
+    </row>
+    <row r="454" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E454" s="2"/>
+    </row>
+    <row r="455" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E455" s="2"/>
+    </row>
+    <row r="456" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E456" s="2"/>
+    </row>
+    <row r="457" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E457" s="2"/>
+    </row>
+    <row r="458" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E458" s="2"/>
+    </row>
+    <row r="459" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E459" s="2"/>
+    </row>
+    <row r="460" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E460" s="2"/>
+    </row>
+    <row r="461" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E461" s="2"/>
+    </row>
+    <row r="462" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E462" s="2"/>
+    </row>
+    <row r="463" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E463" s="2"/>
+    </row>
+    <row r="464" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E464" s="2"/>
+    </row>
+    <row r="465" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E465" s="2"/>
+    </row>
+    <row r="466" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E466" s="2"/>
+    </row>
+    <row r="467" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E467" s="2"/>
+    </row>
+    <row r="468" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E468" s="2"/>
+    </row>
+    <row r="469" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E469" s="2"/>
+    </row>
+    <row r="470" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E470" s="2"/>
+    </row>
+    <row r="471" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E471" s="2"/>
+    </row>
+    <row r="472" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E472" s="2"/>
+    </row>
+    <row r="473" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E473" s="2"/>
+    </row>
+    <row r="474" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E474" s="2"/>
+    </row>
+    <row r="475" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E475" s="2"/>
+    </row>
+    <row r="476" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E476" s="2"/>
+    </row>
+    <row r="477" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E477" s="2"/>
+    </row>
+    <row r="478" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E478" s="2"/>
+    </row>
+    <row r="479" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E479" s="2"/>
+    </row>
+    <row r="480" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E480" s="2"/>
+    </row>
+    <row r="481" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E481" s="2"/>
+    </row>
+    <row r="482" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E482" s="2"/>
+    </row>
+    <row r="483" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E483" s="2"/>
+    </row>
+    <row r="484" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E484" s="2"/>
+    </row>
+    <row r="485" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E485" s="2"/>
+    </row>
+    <row r="486" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E486" s="2"/>
+    </row>
+    <row r="487" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E487" s="2"/>
+    </row>
+    <row r="488" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E488" s="2"/>
+    </row>
+    <row r="489" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E489" s="2"/>
+    </row>
+    <row r="490" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E490" s="2"/>
+    </row>
+    <row r="491" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E491" s="2"/>
+    </row>
+    <row r="492" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E492" s="2"/>
+    </row>
+    <row r="493" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E493" s="2"/>
+    </row>
+    <row r="494" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E494" s="2"/>
+    </row>
+    <row r="495" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E495" s="2"/>
+    </row>
+    <row r="496" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E496" s="2"/>
+    </row>
+    <row r="497" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E497" s="2"/>
+    </row>
+    <row r="498" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E498" s="2"/>
+    </row>
+    <row r="499" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E499" s="2"/>
+    </row>
+    <row r="500" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E500" s="2"/>
+    </row>
+    <row r="501" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E501" s="2"/>
+    </row>
+    <row r="502" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E502" s="2"/>
+    </row>
+    <row r="503" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E503" s="2"/>
+    </row>
+    <row r="504" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E504" s="2"/>
+    </row>
+    <row r="505" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E505" s="2"/>
+    </row>
+    <row r="506" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E506" s="2"/>
+    </row>
+    <row r="507" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E507" s="2"/>
+    </row>
+    <row r="508" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E508" s="2"/>
+    </row>
+    <row r="509" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E509" s="2"/>
+    </row>
+    <row r="510" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E510" s="2"/>
+    </row>
+    <row r="511" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E511" s="2"/>
+    </row>
+    <row r="512" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E512" s="2"/>
+    </row>
+    <row r="513" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E513" s="2"/>
+    </row>
+    <row r="514" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E514" s="2"/>
+    </row>
+    <row r="515" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E515" s="2"/>
+    </row>
+    <row r="516" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E516" s="2"/>
+    </row>
+    <row r="517" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E517" s="2"/>
+    </row>
+    <row r="518" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E518" s="2"/>
+    </row>
+    <row r="519" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E519" s="2"/>
+    </row>
+    <row r="520" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E520" s="2"/>
+    </row>
+    <row r="521" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E521" s="2"/>
+    </row>
+    <row r="522" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E522" s="2"/>
+    </row>
+    <row r="523" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E523" s="2"/>
+    </row>
+    <row r="524" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E524" s="2"/>
+    </row>
+    <row r="525" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E525" s="2"/>
+    </row>
+    <row r="526" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E526" s="2"/>
+    </row>
+    <row r="527" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E527" s="2"/>
+    </row>
+    <row r="528" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E528" s="2"/>
+    </row>
+    <row r="529" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E529" s="2"/>
+    </row>
+    <row r="530" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E530" s="2"/>
+    </row>
+    <row r="531" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E531" s="2"/>
+    </row>
+    <row r="532" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E532" s="2"/>
+    </row>
+    <row r="533" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E533" s="2"/>
+    </row>
+    <row r="534" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E534" s="2"/>
+    </row>
+    <row r="535" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E535" s="2"/>
+    </row>
+    <row r="536" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E536" s="2"/>
+    </row>
+    <row r="537" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E537" s="2"/>
+    </row>
+    <row r="538" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E538" s="2"/>
+    </row>
+    <row r="539" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E539" s="2"/>
+    </row>
+    <row r="540" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E540" s="2"/>
+    </row>
+    <row r="541" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E541" s="2"/>
+    </row>
+    <row r="542" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E542" s="2"/>
+    </row>
+    <row r="543" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E543" s="2"/>
+    </row>
+    <row r="544" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E544" s="2"/>
+    </row>
+    <row r="545" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E545" s="2"/>
+    </row>
+    <row r="546" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E546" s="2"/>
+    </row>
+    <row r="547" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E547" s="2"/>
+    </row>
+    <row r="548" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E548" s="2"/>
+    </row>
+    <row r="549" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E549" s="2"/>
+    </row>
+    <row r="550" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E550" s="2"/>
+    </row>
+    <row r="551" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E551" s="2"/>
+    </row>
+    <row r="552" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E552" s="2"/>
+    </row>
+    <row r="553" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E553" s="2"/>
+    </row>
+    <row r="554" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E554" s="2"/>
+    </row>
+    <row r="555" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E555" s="2"/>
+    </row>
+    <row r="556" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E556" s="2"/>
+    </row>
+    <row r="557" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E557" s="2"/>
+    </row>
+    <row r="558" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E558" s="2"/>
+    </row>
+    <row r="559" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E559" s="2"/>
+    </row>
+    <row r="560" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E560" s="2"/>
+    </row>
+    <row r="561" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E561" s="2"/>
+    </row>
+    <row r="562" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E562" s="2"/>
+    </row>
+    <row r="563" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E563" s="2"/>
+    </row>
+    <row r="564" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E564" s="2"/>
+    </row>
+    <row r="565" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E565" s="2"/>
+    </row>
+    <row r="566" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E566" s="2"/>
+    </row>
+    <row r="567" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E567" s="2"/>
+    </row>
+    <row r="568" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E568" s="2"/>
+    </row>
+    <row r="569" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E569" s="2"/>
+    </row>
+    <row r="570" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E570" s="2"/>
+    </row>
+    <row r="571" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E571" s="2"/>
+    </row>
+    <row r="572" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E572" s="2"/>
+    </row>
+    <row r="573" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E573" s="2"/>
+    </row>
+    <row r="574" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E574" s="2"/>
+    </row>
+    <row r="575" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E575" s="2"/>
+    </row>
+    <row r="576" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E576" s="2"/>
+    </row>
+    <row r="577" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E577" s="2"/>
+    </row>
+    <row r="578" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E578" s="2"/>
+    </row>
+    <row r="579" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E579" s="2"/>
+    </row>
+    <row r="580" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E580" s="2"/>
+    </row>
+    <row r="581" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E581" s="2"/>
+    </row>
+    <row r="582" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E582" s="2"/>
+    </row>
+    <row r="583" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E583" s="2"/>
+    </row>
+    <row r="584" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E584" s="2"/>
+    </row>
+    <row r="585" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E585" s="2"/>
+    </row>
+    <row r="586" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E586" s="2"/>
+    </row>
+    <row r="587" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E587" s="2"/>
+    </row>
+    <row r="588" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E588" s="2"/>
+    </row>
+    <row r="589" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E589" s="2"/>
+    </row>
+    <row r="590" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E590" s="2"/>
+    </row>
+    <row r="591" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E591" s="2"/>
+    </row>
+    <row r="592" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E592" s="2"/>
+    </row>
+    <row r="593" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E593" s="2"/>
+    </row>
+    <row r="594" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E594" s="2"/>
+    </row>
+    <row r="595" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E595" s="2"/>
+    </row>
+    <row r="596" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E596" s="2"/>
+    </row>
+    <row r="597" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E597" s="2"/>
+    </row>
+    <row r="598" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E598" s="2"/>
+    </row>
+    <row r="599" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E599" s="2"/>
+    </row>
+    <row r="600" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E600" s="2"/>
+    </row>
+    <row r="601" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E601" s="2"/>
+    </row>
+    <row r="602" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E602" s="2"/>
+    </row>
+    <row r="603" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E603" s="2"/>
+    </row>
+    <row r="604" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E604" s="2"/>
+    </row>
+    <row r="605" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E605" s="2"/>
+    </row>
+    <row r="606" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E606" s="2"/>
+    </row>
+    <row r="607" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E607" s="2"/>
+    </row>
+    <row r="608" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E608" s="2"/>
+    </row>
+    <row r="609" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E609" s="2"/>
+    </row>
+    <row r="610" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E610" s="2"/>
+    </row>
+    <row r="611" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E611" s="2"/>
+    </row>
+    <row r="612" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E612" s="2"/>
+    </row>
+    <row r="613" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E613" s="2"/>
+    </row>
+    <row r="614" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E614" s="2"/>
+    </row>
+    <row r="615" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E615" s="2"/>
+    </row>
+    <row r="616" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E616" s="2"/>
+    </row>
+    <row r="617" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E617" s="2"/>
+    </row>
+    <row r="618" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E618" s="2"/>
+    </row>
+    <row r="619" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E619" s="2"/>
+    </row>
+    <row r="620" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E620" s="2"/>
+    </row>
+    <row r="621" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E621" s="2"/>
+    </row>
+    <row r="622" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E622" s="2"/>
+    </row>
+    <row r="623" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E623" s="2"/>
+    </row>
+    <row r="624" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E624" s="2"/>
+    </row>
+    <row r="625" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E625" s="2"/>
+    </row>
+    <row r="626" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E626" s="2"/>
+    </row>
+    <row r="627" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E627" s="2"/>
+    </row>
+    <row r="628" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E628" s="2"/>
+    </row>
+    <row r="629" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E629" s="2"/>
+    </row>
+    <row r="630" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E630" s="2"/>
+    </row>
+    <row r="631" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E631" s="2"/>
+    </row>
+    <row r="632" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E632" s="2"/>
+    </row>
+    <row r="633" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E633" s="2"/>
+    </row>
+    <row r="634" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E634" s="2"/>
+    </row>
+    <row r="635" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E635" s="2"/>
+    </row>
+    <row r="636" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E636" s="2"/>
+    </row>
+    <row r="637" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E637" s="2"/>
+    </row>
+    <row r="638" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E638" s="2"/>
+    </row>
+    <row r="639" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E639" s="2"/>
+    </row>
+    <row r="640" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E640" s="2"/>
+    </row>
+    <row r="641" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E641" s="2"/>
+    </row>
+    <row r="642" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E642" s="2"/>
+    </row>
+    <row r="643" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E643" s="2"/>
+    </row>
+    <row r="644" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E644" s="2"/>
+    </row>
+    <row r="645" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E645" s="2"/>
+    </row>
+    <row r="646" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E646" s="2"/>
+    </row>
+    <row r="647" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E647" s="2"/>
+    </row>
+    <row r="648" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E648" s="2"/>
+    </row>
+    <row r="649" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E649" s="2"/>
+    </row>
+    <row r="650" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E650" s="2"/>
+    </row>
+    <row r="651" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E651" s="2"/>
+    </row>
+    <row r="652" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E652" s="2"/>
+    </row>
+    <row r="653" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E653" s="2"/>
+    </row>
+    <row r="654" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E654" s="2"/>
+    </row>
+    <row r="655" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E655" s="2"/>
+    </row>
+    <row r="656" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E656" s="2"/>
+    </row>
+    <row r="657" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E657" s="2"/>
+    </row>
+    <row r="658" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E658" s="2"/>
+    </row>
+    <row r="659" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E659" s="2"/>
+    </row>
+    <row r="660" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E660" s="2"/>
+    </row>
+    <row r="661" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E661" s="2"/>
+    </row>
+    <row r="662" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E662" s="2"/>
+    </row>
+    <row r="663" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E663" s="2"/>
+    </row>
+    <row r="664" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E664" s="2"/>
+    </row>
+    <row r="665" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E665" s="2"/>
+    </row>
+    <row r="666" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E666" s="2"/>
+    </row>
+    <row r="667" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E667" s="2"/>
+    </row>
+    <row r="668" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E668" s="2"/>
+    </row>
+    <row r="669" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E669" s="2"/>
+    </row>
+    <row r="670" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E670" s="2"/>
+    </row>
+    <row r="671" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E671" s="2"/>
+    </row>
+    <row r="672" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E672" s="2"/>
+    </row>
+    <row r="673" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E673" s="2"/>
+    </row>
+    <row r="674" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E674" s="2"/>
+    </row>
+    <row r="675" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E675" s="2"/>
+    </row>
+    <row r="676" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E676" s="2"/>
+    </row>
+    <row r="677" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E677" s="2"/>
+    </row>
+    <row r="678" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E678" s="2"/>
+    </row>
+    <row r="679" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E679" s="2"/>
+    </row>
+    <row r="680" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E680" s="2"/>
+    </row>
+    <row r="681" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E681" s="2"/>
+    </row>
+    <row r="682" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E682" s="2"/>
+    </row>
+    <row r="683" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E683" s="2"/>
+    </row>
+    <row r="684" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E684" s="2"/>
+    </row>
+    <row r="685" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E685" s="2"/>
+    </row>
+    <row r="686" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E686" s="2"/>
+    </row>
+    <row r="687" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E687" s="2"/>
+    </row>
+    <row r="688" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E688" s="2"/>
+    </row>
+    <row r="689" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E689" s="2"/>
+    </row>
+    <row r="690" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E690" s="2"/>
+    </row>
+    <row r="691" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E691" s="2"/>
+    </row>
+    <row r="692" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E692" s="2"/>
+    </row>
+    <row r="693" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E693" s="2"/>
+    </row>
+    <row r="694" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E694" s="2"/>
+    </row>
+    <row r="695" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E695" s="2"/>
+    </row>
+    <row r="696" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E696" s="2"/>
+    </row>
+    <row r="697" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E697" s="2"/>
+    </row>
+    <row r="698" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E698" s="2"/>
+    </row>
+    <row r="699" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E699" s="2"/>
+    </row>
+    <row r="700" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E700" s="2"/>
+    </row>
+    <row r="701" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E701" s="2"/>
+    </row>
+    <row r="702" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E702" s="2"/>
+    </row>
+    <row r="703" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E703" s="2"/>
+    </row>
+    <row r="704" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E704" s="2"/>
+    </row>
+    <row r="705" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E705" s="2"/>
+    </row>
+    <row r="706" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E706" s="2"/>
+    </row>
+    <row r="707" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E707" s="2"/>
+    </row>
+    <row r="708" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E708" s="2"/>
+    </row>
+    <row r="709" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E709" s="2"/>
+    </row>
+    <row r="710" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E710" s="2"/>
+    </row>
+    <row r="711" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E711" s="2"/>
+    </row>
+    <row r="712" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E712" s="2"/>
+    </row>
+    <row r="713" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E713" s="2"/>
+    </row>
+    <row r="714" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E714" s="2"/>
+    </row>
+    <row r="715" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E715" s="2"/>
+    </row>
+    <row r="716" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E716" s="2"/>
+    </row>
+    <row r="717" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E717" s="2"/>
+    </row>
+    <row r="718" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E718" s="2"/>
+    </row>
+    <row r="719" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E719" s="2"/>
+    </row>
+    <row r="720" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E720" s="2"/>
+    </row>
+    <row r="721" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E721" s="2"/>
+    </row>
+    <row r="722" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E722" s="2"/>
+    </row>
+    <row r="723" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E723" s="2"/>
+    </row>
+    <row r="724" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E724" s="2"/>
+    </row>
+    <row r="725" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E725" s="2"/>
+    </row>
+    <row r="726" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E726" s="2"/>
+    </row>
+    <row r="727" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E727" s="2"/>
+    </row>
+    <row r="728" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E728" s="2"/>
+    </row>
+    <row r="729" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E729" s="2"/>
+    </row>
+    <row r="730" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E730" s="2"/>
+    </row>
+    <row r="731" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E731" s="2"/>
+    </row>
+    <row r="732" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E732" s="2"/>
+    </row>
+    <row r="733" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E733" s="2"/>
+    </row>
+    <row r="734" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E734" s="2"/>
+    </row>
+    <row r="735" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E735" s="2"/>
+    </row>
+    <row r="736" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E736" s="2"/>
+    </row>
+    <row r="737" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E737" s="2"/>
+    </row>
+    <row r="738" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E738" s="2"/>
+    </row>
+    <row r="739" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E739" s="2"/>
+    </row>
+    <row r="740" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E740" s="2"/>
+    </row>
+    <row r="741" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E741" s="2"/>
+    </row>
+    <row r="742" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E742" s="2"/>
+    </row>
+    <row r="743" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E743" s="2"/>
+    </row>
+    <row r="744" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E744" s="2"/>
+    </row>
+    <row r="745" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E745" s="2"/>
+    </row>
+    <row r="746" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E746" s="2"/>
+    </row>
+    <row r="747" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E747" s="2"/>
+    </row>
+    <row r="748" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E748" s="2"/>
+    </row>
+    <row r="749" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E749" s="2"/>
+    </row>
+    <row r="750" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E750" s="2"/>
+    </row>
+    <row r="751" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E751" s="2"/>
+    </row>
+    <row r="752" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E752" s="2"/>
+    </row>
+    <row r="753" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E753" s="2"/>
+    </row>
+    <row r="754" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E754" s="2"/>
+    </row>
+    <row r="755" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E755" s="2"/>
+    </row>
+    <row r="756" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E756" s="2"/>
+    </row>
+    <row r="757" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E757" s="2"/>
+    </row>
+    <row r="758" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E758" s="2"/>
+    </row>
+    <row r="759" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E759" s="2"/>
+    </row>
+    <row r="760" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E760" s="2"/>
+    </row>
+    <row r="761" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E761" s="2"/>
+    </row>
+    <row r="762" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E762" s="2"/>
+    </row>
+    <row r="763" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E763" s="2"/>
+    </row>
+    <row r="764" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E764" s="2"/>
+    </row>
+    <row r="765" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E765" s="2"/>
+    </row>
+    <row r="766" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E766" s="2"/>
+    </row>
+    <row r="767" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E767" s="2"/>
+    </row>
+    <row r="768" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E768" s="2"/>
+    </row>
+    <row r="769" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E769" s="2"/>
+    </row>
+    <row r="770" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E770" s="2"/>
+    </row>
+    <row r="771" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E771" s="2"/>
+    </row>
+    <row r="772" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E772" s="2"/>
+    </row>
+    <row r="773" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E773" s="2"/>
+    </row>
+    <row r="774" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E774" s="2"/>
+    </row>
+    <row r="775" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E775" s="2"/>
+    </row>
+    <row r="776" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E776" s="2"/>
+    </row>
+    <row r="777" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E777" s="2"/>
+    </row>
+    <row r="778" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E778" s="2"/>
+    </row>
+    <row r="779" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E779" s="2"/>
+    </row>
+    <row r="780" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E780" s="2"/>
+    </row>
+    <row r="781" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E781" s="2"/>
+    </row>
+    <row r="782" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E782" s="2"/>
+    </row>
+    <row r="783" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E783" s="2"/>
+    </row>
+    <row r="784" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E784" s="2"/>
+    </row>
+    <row r="785" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E785" s="2"/>
+    </row>
+    <row r="786" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E786" s="2"/>
+    </row>
+    <row r="787" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E787" s="2"/>
+    </row>
+    <row r="788" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E788" s="2"/>
+    </row>
+    <row r="789" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E789" s="2"/>
+    </row>
+    <row r="790" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E790" s="2"/>
+    </row>
+    <row r="791" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E791" s="2"/>
+    </row>
+    <row r="792" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E792" s="2"/>
+    </row>
+    <row r="793" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E793" s="2"/>
+    </row>
+    <row r="794" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E794" s="2"/>
+    </row>
+    <row r="795" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E795" s="2"/>
+    </row>
+    <row r="796" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E796" s="2"/>
+    </row>
+    <row r="797" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E797" s="2"/>
+    </row>
+    <row r="798" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E798" s="2"/>
+    </row>
+    <row r="799" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E799" s="2"/>
+    </row>
+    <row r="800" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E800" s="2"/>
+    </row>
+    <row r="801" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E801" s="2"/>
+    </row>
+    <row r="802" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E802" s="2"/>
+    </row>
+    <row r="803" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E803" s="2"/>
+    </row>
+    <row r="804" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E804" s="2"/>
+    </row>
+    <row r="805" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E805" s="2"/>
+    </row>
+    <row r="806" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E806" s="2"/>
+    </row>
+    <row r="807" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E807" s="2"/>
+    </row>
+    <row r="808" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E808" s="2"/>
+    </row>
+    <row r="809" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E809" s="2"/>
+    </row>
+    <row r="810" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E810" s="2"/>
+    </row>
+    <row r="811" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E811" s="2"/>
+    </row>
+    <row r="812" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E812" s="2"/>
+    </row>
+    <row r="813" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E813" s="2"/>
+    </row>
+    <row r="814" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E814" s="2"/>
+    </row>
+    <row r="815" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E815" s="2"/>
+    </row>
+    <row r="816" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E816" s="2"/>
+    </row>
+    <row r="817" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E817" s="2"/>
+    </row>
+    <row r="818" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E818" s="2"/>
+    </row>
+    <row r="819" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E819" s="2"/>
+    </row>
+    <row r="820" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E820" s="2"/>
+    </row>
+    <row r="821" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E821" s="2"/>
+    </row>
+    <row r="822" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E822" s="2"/>
+    </row>
+    <row r="823" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E823" s="2"/>
+    </row>
+    <row r="824" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E824" s="2"/>
+    </row>
+    <row r="825" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E825" s="2"/>
+    </row>
+    <row r="826" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E826" s="2"/>
+    </row>
+    <row r="827" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E827" s="2"/>
+    </row>
+    <row r="828" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E828" s="2"/>
+    </row>
+    <row r="829" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E829" s="2"/>
+    </row>
+    <row r="830" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E830" s="2"/>
+    </row>
+    <row r="831" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E831" s="2"/>
+    </row>
+    <row r="832" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E832" s="2"/>
+    </row>
+    <row r="833" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E833" s="2"/>
+    </row>
+    <row r="834" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E834" s="2"/>
+    </row>
+    <row r="835" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E835" s="2"/>
+    </row>
+    <row r="836" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E836" s="2"/>
+    </row>
+    <row r="837" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E837" s="2"/>
+    </row>
+    <row r="838" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E838" s="2"/>
+    </row>
+    <row r="839" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E839" s="2"/>
+    </row>
+    <row r="840" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E840" s="2"/>
+    </row>
+    <row r="841" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E841" s="2"/>
+    </row>
+    <row r="842" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E842" s="2"/>
+    </row>
+    <row r="843" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E843" s="2"/>
+    </row>
+    <row r="844" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E844" s="2"/>
+    </row>
+    <row r="845" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E845" s="2"/>
+    </row>
+    <row r="846" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E846" s="2"/>
+    </row>
+    <row r="847" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E847" s="2"/>
+    </row>
+    <row r="848" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E848" s="2"/>
+    </row>
+    <row r="849" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E849" s="2"/>
+    </row>
+    <row r="850" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E850" s="2"/>
+    </row>
+    <row r="851" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E851" s="2"/>
+    </row>
+    <row r="852" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E852" s="2"/>
+    </row>
+    <row r="853" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E853" s="2"/>
+    </row>
+    <row r="854" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E854" s="2"/>
+    </row>
+    <row r="855" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E855" s="2"/>
+    </row>
+    <row r="856" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E856" s="2"/>
+    </row>
+    <row r="857" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E857" s="2"/>
+    </row>
+    <row r="858" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E858" s="2"/>
+    </row>
+    <row r="859" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E859" s="2"/>
+    </row>
+    <row r="860" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E860" s="2"/>
+    </row>
+    <row r="861" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E861" s="2"/>
+    </row>
+    <row r="862" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E862" s="2"/>
+    </row>
+    <row r="863" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E863" s="2"/>
+    </row>
+    <row r="864" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E864" s="2"/>
+    </row>
+    <row r="865" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E865" s="2"/>
+    </row>
+    <row r="866" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E866" s="2"/>
+    </row>
+    <row r="867" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E867" s="2"/>
+    </row>
+    <row r="868" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E868" s="2"/>
+    </row>
+    <row r="869" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E869" s="2"/>
+    </row>
+    <row r="870" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E870" s="2"/>
+    </row>
+    <row r="871" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E871" s="2"/>
+    </row>
+    <row r="872" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E872" s="2"/>
+    </row>
+    <row r="873" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E873" s="2"/>
+    </row>
+    <row r="874" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E874" s="2"/>
+    </row>
+    <row r="875" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E875" s="2"/>
+    </row>
+    <row r="876" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E876" s="2"/>
+    </row>
+    <row r="877" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E877" s="2"/>
+    </row>
+    <row r="878" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E878" s="2"/>
+    </row>
+    <row r="879" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E879" s="2"/>
+    </row>
+    <row r="880" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E880" s="2"/>
+    </row>
+    <row r="881" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E881" s="2"/>
+    </row>
+    <row r="882" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E882" s="2"/>
+    </row>
+    <row r="883" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E883" s="2"/>
+    </row>
+    <row r="884" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E884" s="2"/>
+    </row>
+    <row r="885" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E885" s="2"/>
+    </row>
+    <row r="886" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E886" s="2"/>
+    </row>
+    <row r="887" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E887" s="2"/>
+    </row>
+    <row r="888" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E888" s="2"/>
+    </row>
+    <row r="889" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E889" s="2"/>
+    </row>
+    <row r="890" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E890" s="2"/>
+    </row>
+    <row r="891" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E891" s="2"/>
+    </row>
+    <row r="892" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E892" s="2"/>
+    </row>
+    <row r="893" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E893" s="2"/>
+    </row>
+    <row r="894" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E894" s="2"/>
+    </row>
+    <row r="895" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E895" s="2"/>
+    </row>
+    <row r="896" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E896" s="2"/>
+    </row>
+    <row r="897" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E897" s="2"/>
+    </row>
+    <row r="898" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E898" s="2"/>
+    </row>
+    <row r="899" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E899" s="2"/>
+    </row>
+    <row r="900" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E900" s="2"/>
+    </row>
+    <row r="901" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E901" s="2"/>
+    </row>
+    <row r="902" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E902" s="2"/>
+    </row>
+    <row r="903" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E903" s="2"/>
+    </row>
+    <row r="904" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E904" s="2"/>
+    </row>
+    <row r="905" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E905" s="2"/>
+    </row>
+    <row r="906" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E906" s="2"/>
+    </row>
+    <row r="907" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E907" s="2"/>
+    </row>
+    <row r="908" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E908" s="2"/>
+    </row>
+    <row r="909" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E909" s="2"/>
+    </row>
+    <row r="910" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E910" s="2"/>
+    </row>
+    <row r="911" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E911" s="2"/>
+    </row>
+    <row r="912" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E912" s="2"/>
+    </row>
+    <row r="913" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E913" s="2"/>
+    </row>
+    <row r="914" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E914" s="2"/>
+    </row>
+    <row r="915" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E915" s="2"/>
+    </row>
+    <row r="916" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E916" s="2"/>
+    </row>
+    <row r="917" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E917" s="2"/>
+    </row>
+    <row r="918" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E918" s="2"/>
+    </row>
+    <row r="919" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E919" s="2"/>
+    </row>
+    <row r="920" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E920" s="2"/>
+    </row>
+    <row r="921" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E921" s="2"/>
+    </row>
+    <row r="922" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E922" s="2"/>
+    </row>
+    <row r="923" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E923" s="2"/>
+    </row>
+    <row r="924" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E924" s="2"/>
+    </row>
+    <row r="925" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E925" s="2"/>
+    </row>
+    <row r="926" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E926" s="2"/>
+    </row>
+    <row r="927" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E927" s="2"/>
+    </row>
+    <row r="928" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E928" s="2"/>
+    </row>
+    <row r="929" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E929" s="2"/>
+    </row>
+    <row r="930" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E930" s="2"/>
+    </row>
+    <row r="931" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E931" s="2"/>
+    </row>
+    <row r="932" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E932" s="2"/>
+    </row>
+    <row r="933" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E933" s="2"/>
+    </row>
+    <row r="934" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E934" s="2"/>
+    </row>
+    <row r="935" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E935" s="2"/>
+    </row>
+    <row r="936" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E936" s="2"/>
+    </row>
+    <row r="937" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E937" s="2"/>
+    </row>
+    <row r="938" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E938" s="2"/>
+    </row>
+    <row r="939" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E939" s="2"/>
+    </row>
+    <row r="940" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E940" s="2"/>
+    </row>
+    <row r="941" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E941" s="2"/>
+    </row>
+    <row r="942" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E942" s="2"/>
+    </row>
+    <row r="943" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E943" s="2"/>
+    </row>
+    <row r="944" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E944" s="2"/>
+    </row>
+    <row r="945" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E945" s="2"/>
+    </row>
+    <row r="946" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E946" s="2"/>
+    </row>
+    <row r="947" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E947" s="2"/>
+    </row>
+    <row r="948" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E948" s="2"/>
+    </row>
+    <row r="949" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E949" s="2"/>
+    </row>
+    <row r="950" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E950" s="2"/>
+    </row>
+    <row r="951" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E951" s="2"/>
+    </row>
+    <row r="952" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E952" s="2"/>
+    </row>
+    <row r="953" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E953" s="2"/>
+    </row>
+    <row r="954" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E954" s="2"/>
+    </row>
+    <row r="955" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E955" s="2"/>
+    </row>
+    <row r="956" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E956" s="2"/>
+    </row>
+    <row r="957" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E957" s="2"/>
+    </row>
+    <row r="958" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E958" s="2"/>
+    </row>
+    <row r="959" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E959" s="2"/>
+    </row>
+    <row r="960" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E960" s="2"/>
+    </row>
+    <row r="961" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E961" s="2"/>
+    </row>
+    <row r="962" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E962" s="2"/>
+    </row>
+    <row r="963" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E963" s="2"/>
+    </row>
+    <row r="964" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E964" s="2"/>
+    </row>
+    <row r="965" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E965" s="2"/>
+    </row>
+    <row r="966" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E966" s="2"/>
+    </row>
+    <row r="967" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E967" s="2"/>
+    </row>
+    <row r="968" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E968" s="2"/>
+    </row>
+    <row r="969" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E969" s="2"/>
+    </row>
+    <row r="970" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E970" s="2"/>
+    </row>
+    <row r="971" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E971" s="2"/>
+    </row>
+    <row r="972" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E972" s="2"/>
+    </row>
+    <row r="973" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E973" s="2"/>
+    </row>
+    <row r="974" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E974" s="2"/>
+    </row>
+    <row r="975" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E975" s="2"/>
+    </row>
+    <row r="976" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E976" s="2"/>
+    </row>
+    <row r="977" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E977" s="2"/>
+    </row>
+    <row r="978" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E978" s="2"/>
+    </row>
+    <row r="979" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E979" s="2"/>
+    </row>
+    <row r="980" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E980" s="2"/>
+    </row>
+    <row r="981" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E981" s="2"/>
+    </row>
+    <row r="982" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E982" s="2"/>
+    </row>
+    <row r="983" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E983" s="2"/>
+    </row>
+    <row r="984" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E984" s="2"/>
+    </row>
+    <row r="985" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E985" s="2"/>
+    </row>
+    <row r="986" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E986" s="2"/>
+    </row>
+    <row r="987" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E987" s="2"/>
+    </row>
+    <row r="988" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E988" s="2"/>
+    </row>
+    <row r="989" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E989" s="2"/>
+    </row>
+    <row r="990" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E990" s="2"/>
+    </row>
+    <row r="991" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E991" s="2"/>
+    </row>
+    <row r="992" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E992" s="2"/>
+    </row>
+    <row r="993" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E993" s="2"/>
+    </row>
+    <row r="994" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E994" s="2"/>
+    </row>
+    <row r="995" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E995" s="2"/>
+    </row>
+    <row r="996" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E996" s="2"/>
+    </row>
+    <row r="997" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E997" s="2"/>
+    </row>
+    <row r="998" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E998" s="2"/>
+    </row>
+    <row r="999" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E999" s="2"/>
+    </row>
+    <row r="1000" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1000" s="2"/>
+    </row>
+    <row r="1001" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1001" s="2"/>
+    </row>
+    <row r="1002" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1002" s="2"/>
+    </row>
+    <row r="1003" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1003" s="2"/>
+    </row>
+    <row r="1004" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1004" s="2"/>
+    </row>
+    <row r="1005" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1005" s="2"/>
+    </row>
+    <row r="1006" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1006" s="2"/>
+    </row>
+    <row r="1007" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1007" s="2"/>
+    </row>
+    <row r="1008" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1008" s="2"/>
+    </row>
+    <row r="1009" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1009" s="2"/>
+    </row>
+    <row r="1010" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1010" s="2"/>
+    </row>
+    <row r="1011" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1011" s="2"/>
+    </row>
+    <row r="1012" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1012" s="2"/>
+    </row>
+    <row r="1013" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1013" s="2"/>
+    </row>
+    <row r="1014" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1014" s="2"/>
+    </row>
+    <row r="1015" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1015" s="2"/>
+    </row>
+    <row r="1016" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1016" s="2"/>
+    </row>
+    <row r="1017" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1017" s="2"/>
+    </row>
+    <row r="1018" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1018" s="2"/>
+    </row>
+    <row r="1019" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1019" s="2"/>
+    </row>
+    <row r="1020" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1020" s="2"/>
+    </row>
+    <row r="1021" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1021" s="2"/>
+    </row>
+    <row r="1022" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1022" s="2"/>
+    </row>
+    <row r="1023" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1023" s="2"/>
+    </row>
+    <row r="1024" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1024" s="2"/>
+    </row>
+    <row r="1025" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1025" s="2"/>
+    </row>
+    <row r="1026" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1026" s="2"/>
+    </row>
+    <row r="1027" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1027" s="2"/>
+    </row>
+    <row r="1028" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1028" s="2"/>
+    </row>
+    <row r="1029" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1029" s="2"/>
+    </row>
+    <row r="1030" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1030" s="2"/>
+    </row>
+    <row r="1031" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1031" s="2"/>
+    </row>
+    <row r="1032" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1032" s="2"/>
+    </row>
+    <row r="1033" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1033" s="2"/>
+    </row>
+    <row r="1034" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1034" s="2"/>
+    </row>
+    <row r="1035" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1035" s="2"/>
+    </row>
+    <row r="1036" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1036" s="2"/>
+    </row>
+    <row r="1037" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1037" s="2"/>
+    </row>
+    <row r="1038" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1038" s="2"/>
+    </row>
+    <row r="1039" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1039" s="2"/>
+    </row>
+    <row r="1040" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1040" s="2"/>
+    </row>
+    <row r="1041" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1041" s="2"/>
+    </row>
+    <row r="1042" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1042" s="2"/>
+    </row>
+    <row r="1043" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1043" s="2"/>
+    </row>
+    <row r="1044" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1044" s="2"/>
+    </row>
+    <row r="1045" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1045" s="2"/>
+    </row>
+    <row r="1046" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1046" s="2"/>
+    </row>
+    <row r="1047" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1047" s="2"/>
+    </row>
+    <row r="1048" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1048" s="2"/>
+    </row>
+    <row r="1049" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1049" s="2"/>
+    </row>
+    <row r="1050" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1050" s="2"/>
+    </row>
+    <row r="1051" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1051" s="2"/>
+    </row>
+    <row r="1052" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1052" s="2"/>
+    </row>
+    <row r="1053" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1053" s="2"/>
+    </row>
+    <row r="1054" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1054" s="2"/>
+    </row>
+    <row r="1055" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1055" s="2"/>
+    </row>
+    <row r="1056" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1056" s="2"/>
+    </row>
+    <row r="1057" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1057" s="2"/>
+    </row>
+    <row r="1058" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1058" s="2"/>
+    </row>
+    <row r="1059" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1059" s="2"/>
+    </row>
+    <row r="1060" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1060" s="2"/>
+    </row>
+    <row r="1061" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1061" s="2"/>
+    </row>
+    <row r="1062" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1062" s="2"/>
+    </row>
+    <row r="1063" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1063" s="2"/>
+    </row>
+    <row r="1064" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1064" s="2"/>
+    </row>
+    <row r="1065" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1065" s="2"/>
+    </row>
+    <row r="1066" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1066" s="2"/>
+    </row>
+    <row r="1067" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1067" s="2"/>
+    </row>
+    <row r="1068" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1068" s="2"/>
+    </row>
+    <row r="1069" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1069" s="2"/>
+    </row>
+    <row r="1070" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1070" s="2"/>
+    </row>
+    <row r="1071" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1071" s="2"/>
+    </row>
+    <row r="1072" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1072" s="2"/>
+    </row>
+    <row r="1073" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1073" s="2"/>
+    </row>
+    <row r="1074" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1074" s="2"/>
+    </row>
+    <row r="1075" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1075" s="2"/>
+    </row>
+    <row r="1076" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1076" s="2"/>
+    </row>
+    <row r="1077" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1077" s="2"/>
+    </row>
+    <row r="1078" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1078" s="2"/>
+    </row>
+    <row r="1079" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1079" s="2"/>
+    </row>
+    <row r="1080" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1080" s="2"/>
+    </row>
+    <row r="1081" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1081" s="2"/>
+    </row>
+    <row r="1082" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1082" s="2"/>
+    </row>
+    <row r="1083" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1083" s="2"/>
+    </row>
+    <row r="1084" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1084" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1000">
       <formula1>"Conter as palavras,For igual"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000">
       <formula1>"Fornecedor,Plano de Contas,Categoria,Histórico"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1084">
+      <formula1>"Sim,Não"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -524,7 +3783,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: update sheet configuracoes and add read proofs sicoob
</commit_message>
<xml_diff>
--- a/backend/accounting_integration/data/configuracoes.xlsx
+++ b/backend/accounting_integration/data/configuracoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-945" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-20610" yWindow="-945" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FornecedorOuDespesa" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
   <dimension ref="A1:E1084"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -3781,7 +3781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
@@ -3826,9 +3826,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: implement ofx feats and Proofsamazonia
</commit_message>
<xml_diff>
--- a/backend/accounting_integration/data/configuracoes.xlsx
+++ b/backend/accounting_integration/data/configuracoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-945" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-20610" yWindow="-945" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="FornecedorOuDespesa" sheetId="1" r:id="rId1"/>
@@ -480,9 +480,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1084"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3826,7 +3826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>

</xml_diff>